<commit_message>
Calificaciones practicas 3 y 4
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
   <si>
     <t xml:space="preserve">Coordinación de Ciencias Cognitivas y del Comportamiento</t>
   </si>
@@ -58,10 +58,19 @@
     <t xml:space="preserve">Grupo</t>
   </si>
   <si>
+    <t xml:space="preserve">Promedio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Práctica psicofísica</t>
   </si>
   <si>
     <t xml:space="preserve">Práctica escucha dicótica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Práctica Efecto Stroop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mágico número 7</t>
   </si>
   <si>
     <t xml:space="preserve">ARRIETA</t>
@@ -501,8 +510,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -514,7 +523,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -594,7 +603,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -671,40 +680,59 @@
       <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="J5" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="K5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>422043029</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H6" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I6" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">AVERAGE(K6:N6)</f>
+        <v>9.2</v>
       </c>
       <c r="K6" s="10" t="n">
         <v>8.6</v>
@@ -712,34 +740,50 @@
       <c r="L6" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E7" s="9" t="n">
         <v>96575404</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H7" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I7" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">AVERAGE(K7:N7)</f>
+        <v>9.2</v>
       </c>
       <c r="K7" s="10" t="n">
         <v>8.6</v>
@@ -747,34 +791,50 @@
       <c r="L7" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>3</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>319303177</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H8" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I8" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">AVERAGE(K8:N8)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K8" s="10" t="n">
         <v>7.2</v>
@@ -782,28 +842,38 @@
       <c r="L8" s="10" t="n">
         <v>8.7</v>
       </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="n">
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="9" t="n">
         <v>319332478</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H9" s="9" t="n">
         <v>1400</v>
@@ -811,38 +881,58 @@
       <c r="I9" s="9" t="n">
         <v>4108</v>
       </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">AVERAGE(K9:N9)</f>
+        <v>8.83333333333333</v>
+      </c>
       <c r="K9" s="10" t="n">
         <v>9</v>
       </c>
       <c r="L9" s="10"/>
+      <c r="M9" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="n">
         <v>5</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" s="9" t="n">
         <v>319146592</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H10" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I10" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">AVERAGE(K10:N10)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K10" s="10" t="n">
         <v>7.2</v>
@@ -850,34 +940,48 @@
       <c r="L10" s="10" t="n">
         <v>8.7</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="7"/>
+      <c r="N10" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="n">
         <v>6</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E11" s="9" t="n">
         <v>319275230</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H11" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I11" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">AVERAGE(K11:N11)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K11" s="10" t="n">
         <v>7.2</v>
@@ -885,34 +989,48 @@
       <c r="L11" s="10" t="n">
         <v>8.7</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="7"/>
+      <c r="N11" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="n">
         <v>7</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E12" s="9" t="n">
         <v>319043226</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H12" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I12" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">AVERAGE(K12:N12)</f>
+        <v>8.9</v>
       </c>
       <c r="K12" s="10" t="n">
         <v>9</v>
@@ -920,34 +1038,46 @@
       <c r="L12" s="10" t="n">
         <v>8.8</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="n">
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13" s="9" t="n">
         <v>319321997</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H13" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I13" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">AVERAGE(K13:N13)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K13" s="10" t="n">
         <v>7.2</v>
@@ -955,34 +1085,48 @@
       <c r="L13" s="10" t="n">
         <v>8.7</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="7"/>
+      <c r="N13" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="n">
         <v>9</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>319231302</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H14" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I14" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">AVERAGE(K14:N14)</f>
+        <v>9.2</v>
       </c>
       <c r="K14" s="10" t="n">
         <v>8.6</v>
@@ -990,34 +1134,50 @@
       <c r="L14" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N14" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
         <v>10</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E15" s="9" t="n">
         <v>319303359</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H15" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I15" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">AVERAGE(K15:N15)</f>
+        <v>9.225</v>
       </c>
       <c r="K15" s="10" t="n">
         <v>9</v>
@@ -1025,34 +1185,50 @@
       <c r="L15" s="10" t="n">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N15" s="7" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="n">
         <v>11</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E16" s="9" t="n">
         <v>319205930</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H16" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I16" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">AVERAGE(K16:N16)</f>
+        <v>8.96666666666667</v>
       </c>
       <c r="K16" s="10" t="n">
         <v>9</v>
@@ -1060,34 +1236,48 @@
       <c r="L16" s="10" t="n">
         <v>8.8</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="n">
         <v>12</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E17" s="9" t="n">
         <v>319205947</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H17" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I17" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">AVERAGE(K17:N17)</f>
+        <v>9.2</v>
       </c>
       <c r="K17" s="10" t="n">
         <v>8.6</v>
@@ -1095,34 +1285,50 @@
       <c r="L17" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N17" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="n">
         <v>13</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E18" s="9" t="n">
         <v>318311001</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H18" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I18" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">AVERAGE(K18:N18)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K18" s="10" t="n">
         <v>7.2</v>
@@ -1130,34 +1336,48 @@
       <c r="L18" s="10" t="n">
         <v>8.7</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="7"/>
+      <c r="N18" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="n">
         <v>14</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E19" s="9" t="n">
         <v>319280276</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H19" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I19" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">AVERAGE(K19:N19)</f>
+        <v>8.26666666666667</v>
       </c>
       <c r="K19" s="10" t="n">
         <v>7.2</v>
@@ -1165,34 +1385,48 @@
       <c r="L19" s="10" t="n">
         <v>8.7</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="7"/>
+      <c r="N19" s="7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="n">
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E20" s="9" t="n">
         <v>319084146</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H20" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I20" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">AVERAGE(K20:N20)</f>
+        <v>8.96666666666667</v>
       </c>
       <c r="K20" s="10" t="n">
         <v>9</v>
@@ -1200,28 +1434,38 @@
       <c r="L20" s="10" t="n">
         <v>8.8</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="n">
         <v>16</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>319294215</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H21" s="9" t="n">
         <v>1400</v>
@@ -1229,32 +1473,48 @@
       <c r="I21" s="9" t="n">
         <v>4108</v>
       </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">AVERAGE(K21:N21)</f>
+        <v>8.83333333333333</v>
+      </c>
       <c r="K21" s="10" t="n">
         <v>9</v>
       </c>
       <c r="L21" s="10"/>
-    </row>
-    <row r="22" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="N21" s="7" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="n">
         <v>17</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E22" s="9" t="n">
         <v>319321629</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H22" s="9" t="n">
         <v>1400</v>
@@ -1262,32 +1522,48 @@
       <c r="I22" s="9" t="n">
         <v>4108</v>
       </c>
+      <c r="J22" s="0" t="n">
+        <f aca="false">AVERAGE(K22:N22)</f>
+        <v>8.83333333333333</v>
+      </c>
       <c r="K22" s="10" t="n">
         <v>9</v>
       </c>
       <c r="L22" s="10"/>
-    </row>
-    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="N22" s="7" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="n">
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E23" s="9" t="n">
         <v>319023653</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H23" s="9" t="n">
         <v>1400</v>
@@ -1295,69 +1571,101 @@
       <c r="I23" s="9" t="n">
         <v>4108</v>
       </c>
+      <c r="J23" s="0" t="n">
+        <f aca="false">AVERAGE(K23:N23)</f>
+        <v>8.83333333333333</v>
+      </c>
       <c r="K23" s="10" t="n">
         <v>9</v>
       </c>
       <c r="L23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="N23" s="7" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="n">
         <v>19</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E24" s="9" t="n">
         <v>422128740</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H24" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I24" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J24" s="0" t="e">
+        <f aca="false">AVERAGE(K24:N24)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="n">
         <v>20</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E25" s="9" t="n">
         <v>319120453</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H25" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I25" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <f aca="false">AVERAGE(K25:N25)</f>
+        <v>9.2</v>
       </c>
       <c r="K25" s="10" t="n">
         <v>8.6</v>
@@ -1365,34 +1673,50 @@
       <c r="L25" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M25" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N25" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="n">
         <v>21</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E26" s="9" t="n">
         <v>319306642</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H26" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I26" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">AVERAGE(K26:N26)</f>
+        <v>8.96666666666667</v>
       </c>
       <c r="K26" s="10" t="n">
         <v>9</v>
@@ -1400,34 +1724,48 @@
       <c r="L26" s="10" t="n">
         <v>8.8</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="n">
         <v>22</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E27" s="9" t="n">
         <v>319175408</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H27" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I27" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">AVERAGE(K27:N27)</f>
+        <v>8.96666666666667</v>
       </c>
       <c r="K27" s="10" t="n">
         <v>9</v>
@@ -1435,34 +1773,48 @@
       <c r="L27" s="10" t="n">
         <v>8.8</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M27" s="7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="n">
         <v>23</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E28" s="9" t="n">
         <v>421048045</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H28" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I28" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <f aca="false">AVERAGE(K28:N28)</f>
+        <v>9.225</v>
       </c>
       <c r="K28" s="10" t="n">
         <v>9</v>
@@ -1470,34 +1822,50 @@
       <c r="L28" s="10" t="n">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M28" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N28" s="7" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="n">
         <v>24</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E29" s="9" t="n">
         <v>319041882</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H29" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I29" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <f aca="false">AVERAGE(K29:N29)</f>
+        <v>9.2</v>
       </c>
       <c r="K29" s="10" t="n">
         <v>8.6</v>
@@ -1505,34 +1873,50 @@
       <c r="L29" s="10" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M29" s="7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N29" s="7" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="n">
         <v>25</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E30" s="9" t="n">
         <v>319063758</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H30" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I30" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <f aca="false">AVERAGE(K30:N30)</f>
+        <v>9.225</v>
       </c>
       <c r="K30" s="10" t="n">
         <v>9</v>
@@ -1540,34 +1924,50 @@
       <c r="L30" s="10" t="n">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M30" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N30" s="7" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="n">
         <v>26</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E31" s="9" t="n">
         <v>319122316</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H31" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I31" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <f aca="false">AVERAGE(K31:N31)</f>
+        <v>9.225</v>
       </c>
       <c r="K31" s="10" t="n">
         <v>9</v>
@@ -1575,28 +1975,40 @@
       <c r="L31" s="10" t="n">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M31" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N31" s="7" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="n">
         <v>27</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E32" s="9" t="n">
         <v>319248744</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H32" s="9" t="n">
         <v>1400</v>
@@ -1604,38 +2016,58 @@
       <c r="I32" s="9" t="n">
         <v>4108</v>
       </c>
+      <c r="J32" s="0" t="n">
+        <f aca="false">AVERAGE(K32:N32)</f>
+        <v>8.83333333333333</v>
+      </c>
       <c r="K32" s="10" t="n">
         <v>9</v>
       </c>
       <c r="L32" s="10"/>
-    </row>
-    <row r="33" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M32" s="7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="N32" s="7" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="n">
         <v>28</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E33" s="9" t="n">
         <v>319227648</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H33" s="9" t="n">
         <v>1400</v>
       </c>
       <c r="I33" s="9" t="n">
         <v>4108</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">AVERAGE(K33:N33)</f>
+        <v>9.225</v>
       </c>
       <c r="K33" s="10" t="n">
         <v>9</v>
@@ -1643,6 +2075,18 @@
       <c r="L33" s="10" t="n">
         <v>9.1</v>
       </c>
+      <c r="M33" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N33" s="7" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>